<commit_message>
home page ui changes
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8749C0-8BE7-402A-AF27-D75C10A80BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AC8F2B-59C0-4B65-9487-C30AA2D100EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E77E95B9-6C72-458A-B6BB-E1A7312116CE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Class</t>
   </si>
@@ -133,6 +133,15 @@
   </si>
   <si>
     <t>Computer</t>
+  </si>
+  <si>
+    <t>LKG</t>
+  </si>
+  <si>
+    <t>Nasim</t>
+  </si>
+  <si>
+    <t>Kamal</t>
   </si>
 </sst>
 </file>
@@ -176,13 +185,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -498,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39A9FEF-C8A2-4DA1-A01D-DD3776233EC9}">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -656,39 +668,39 @@
       </c>
       <c r="F4">
         <f t="shared" ref="F4:N12" ca="1" si="0">RANDBETWEEN(40,100)</f>
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>56</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="0"/>
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="N4">
         <f t="shared" ca="1" si="0"/>
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -709,39 +721,39 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="N5">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -762,39 +774,39 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="0"/>
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="N6">
         <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -815,39 +827,39 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="0"/>
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="N7">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -868,39 +880,39 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ca="1" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ca="1" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ca="1" si="0"/>
+        <v>89</v>
+      </c>
+      <c r="K8">
+        <f t="shared" ca="1" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="L8">
+        <f t="shared" ca="1" si="0"/>
         <v>91</v>
       </c>
-      <c r="H8">
-        <f t="shared" ca="1" si="0"/>
-        <v>79</v>
-      </c>
-      <c r="I8">
-        <f t="shared" ca="1" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="J8">
-        <f t="shared" ca="1" si="0"/>
-        <v>82</v>
-      </c>
-      <c r="K8">
-        <f t="shared" ca="1" si="0"/>
-        <v>71</v>
-      </c>
-      <c r="L8">
-        <f t="shared" ca="1" si="0"/>
-        <v>54</v>
-      </c>
       <c r="M8">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="N8">
         <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -921,31 +933,31 @@
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ca="1" si="0"/>
         <v>60</v>
       </c>
-      <c r="G9">
-        <f t="shared" ca="1" si="0"/>
-        <v>43</v>
-      </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="0"/>
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="M9">
         <f t="shared" ca="1" si="0"/>
@@ -953,7 +965,7 @@
       </c>
       <c r="N9">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -974,39 +986,39 @@
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ca="1" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="I10">
+        <f t="shared" ca="1" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="J10">
+        <f t="shared" ca="1" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="K10">
+        <f t="shared" ca="1" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ca="1" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ca="1" si="0"/>
         <v>78</v>
       </c>
-      <c r="H10">
-        <f t="shared" ca="1" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="I10">
-        <f t="shared" ca="1" si="0"/>
-        <v>97</v>
-      </c>
-      <c r="J10">
-        <f t="shared" ca="1" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="K10">
-        <f t="shared" ca="1" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="L10">
-        <f t="shared" ca="1" si="0"/>
-        <v>99</v>
-      </c>
-      <c r="M10">
-        <f t="shared" ca="1" si="0"/>
-        <v>78</v>
-      </c>
       <c r="N10">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -1027,27 +1039,27 @@
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="0"/>
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="L11">
         <f t="shared" ca="1" si="0"/>
@@ -1059,7 +1071,7 @@
       </c>
       <c r="N11">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
@@ -1080,38 +1092,82 @@
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="L12">
         <f t="shared" ca="1" si="0"/>
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="M12">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="N12">
         <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="2">
+        <v>60</v>
+      </c>
+      <c r="F13">
+        <v>70</v>
+      </c>
+      <c r="G13" s="2">
+        <v>67</v>
+      </c>
+      <c r="H13" s="2">
+        <v>76</v>
+      </c>
+      <c r="I13" s="2">
+        <v>89</v>
+      </c>
+      <c r="J13" s="2">
+        <v>76</v>
+      </c>
+      <c r="K13" s="2">
+        <v>98</v>
+      </c>
+      <c r="L13" s="2">
+        <v>98</v>
+      </c>
+      <c r="M13" s="2">
+        <v>67</v>
+      </c>
+      <c r="N13" s="2">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>